<commit_message>
Ajuste de filtros. Fase 1- LS
</commit_message>
<xml_diff>
--- a/nomes_paraquat.xlsx
+++ b/nomes_paraquat.xlsx
@@ -21,51 +21,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
-  <si>
-    <t xml:space="preserve">“laredo”</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+  <si>
+    <t xml:space="preserve">"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1'-dimethyl-4,4'-bipyridinium</t>
   </si>
   <si>
     <t xml:space="preserve">,</t>
   </si>
   <si>
-    <t xml:space="preserve">“orbit”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“tocha”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“gramocil”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“gramoxone”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“helmoxone”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“paradox”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“pramato”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“gramoking”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“quatdown”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“sprayquat”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“nuquat”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“flak 200”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“paraquat”</t>
+    <t xml:space="preserve">c12h14n2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dicloreto de N,N′-dimetil-4,4′-bipiridínio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bipiridínio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bipyridinium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flak 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gramocil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gramoking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gramoxone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gramoxone 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helmoxone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laredo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuquat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paradox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paraquat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paraquat 200 sl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paraquate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paraquate alta 200 sl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pramato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quatdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprayquat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tocha</t>
   </si>
   <si>
     <t xml:space="preserve">“alamos“,</t>
@@ -182,8 +212,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,6 +234,15 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -314,180 +357,447 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.18"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A1,B1)</f>
-        <v>“laredo”,</v>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A1,B1,C1,D1)</f>
+        <v>"1,1'-dimethyl-4,4'-bipyridinium",</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A2,B2)</f>
-        <v>“orbit”,</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A2,B2,C2,D2)</f>
+        <v>"c12h14n2",</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A3,B3)</f>
-        <v>“tocha”,</v>
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A3,B3,C3,D3)</f>
+        <v>"dicloreto de N,N′-dimetil-4,4′-bipiridínio",</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A4,B4)</f>
-        <v>“gramocil”,</v>
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A4,B4,C4,D4)</f>
+        <v>"bipiridínio",</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A5,B5)</f>
-        <v>“gramoxone”,</v>
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A5,B5,C5,D5)</f>
+        <v>"bipyridinium",</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A6,B6)</f>
-        <v>“helmoxone”,</v>
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A6,B6,C6,D6)</f>
+        <v>"flak 200",</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A7,B7)</f>
-        <v>“paradox”,</v>
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A7,B7,C7,D7)</f>
+        <v>"gramocil",</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A8,B8)</f>
-        <v>“pramato”,</v>
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A8,B8,C8,D8)</f>
+        <v>"gramoking",</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A9,B9)</f>
-        <v>“gramoking”,</v>
+      <c r="C9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A9,B9,C9,D9)</f>
+        <v>"gramoking",</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A10,B10)</f>
-        <v>“quatdown”,</v>
+      <c r="C10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A10,B10,C10,D10)</f>
+        <v>"gramoxone",</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A11,B11)</f>
-        <v>“sprayquat”,</v>
+      <c r="C11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A11,B11,C11,D11)</f>
+        <v>"gramoxone 200",</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A12,B12)</f>
-        <v>“nuquat”,</v>
+      <c r="C12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A12,B12,C12,D12)</f>
+        <v>"helmoxone",</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A13,B13)</f>
-        <v>“flak 200”,</v>
+      <c r="C13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A13,B13,C13,D13)</f>
+        <v>"laredo",</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(A14,B14)</f>
-        <v>“paraquat”,</v>
+      <c r="C14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A14,B14,C14,D14)</f>
+        <v>"nuquat",</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A15,B15,C15,D15)</f>
+        <v>"orbit",</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A16,B16,C16,D16)</f>
+        <v>"paradox",</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A17,B17,C17,D17)</f>
+        <v>"paraquat",</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A18,B18,C18,D18)</f>
+        <v>"paraquat 200 sl",</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A19,B19,C19,D19)</f>
+        <v>"paraquate",</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A20,B20,C20,D20)</f>
+        <v>"paraquate alta 200 sl",</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A21,B21,C21,D21)</f>
+        <v>"pramato",</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A22,B22,C22,D22)</f>
+        <v>"quatdown",</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A23,B23,C23,D23)</f>
+        <v>"sprayquat",</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A24,B24,C24,D24)</f>
+        <v>"tocha",</v>
       </c>
     </row>
   </sheetData>
@@ -509,79 +819,79 @@
   <dimension ref="D1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="1" t="s">
-        <v>15</v>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="1" t="s">
-        <v>16</v>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="1" t="s">
-        <v>17</v>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1" t="s">
-        <v>18</v>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="1" t="s">
-        <v>19</v>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="1" t="s">
-        <v>20</v>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="1" t="s">
-        <v>21</v>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="1" t="s">
-        <v>22</v>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="1" t="s">
-        <v>23</v>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="1" t="s">
-        <v>24</v>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="1" t="s">
-        <v>25</v>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="1" t="s">
-        <v>26</v>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="1" t="s">
-        <v>27</v>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="1" t="s">
-        <v>28</v>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>